<commit_message>
added beekeeper and colony numbers from 1990
</commit_message>
<xml_diff>
--- a/data/tables.xlsx
+++ b/data/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/btree-mac/Repos/coloss_austria_colony_losses_zukunftbiene2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BAAB26-0949-4B45-8578-82292BE1A434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B74EC9-315C-3747-917D-5A0C5A7D938A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29900" yWindow="500" windowWidth="35060" windowHeight="18700" activeTab="1" xr2:uid="{3C9A20F8-BFAC-0848-B48A-06BB11FCA9E9}"/>
+    <workbookView xWindow="-30720" yWindow="500" windowWidth="30720" windowHeight="18700" xr2:uid="{3C9A20F8-BFAC-0848-B48A-06BB11FCA9E9}"/>
   </bookViews>
   <sheets>
     <sheet name="beteiligungsrate" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="939">
   <si>
     <t>Jahr </t>
   </si>
@@ -2862,6 +2862,12 @@
   </si>
   <si>
     <t>(59; 819)</t>
+  </si>
+  <si>
+    <t>Anzahl der Imkerinnen und Imker (Imker) und Anzahl der Bienenvölker in Österreich seit 1990. Quelle: BMLRT(1) , FAO(2)</t>
+  </si>
+  <si>
+    <t>Imker</t>
   </si>
 </sst>
 </file>
@@ -3133,33 +3139,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -3185,12 +3164,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3505,10 +3511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5564593E-6785-9649-9B47-6616672015F2}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3521,19 +3527,19 @@
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="56" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70" t="s">
         <v>827</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3555,8 +3561,11 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3579,7 +3588,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3602,7 +3611,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3624,8 +3633,17 @@
       <c r="G5" s="4">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>938</v>
+      </c>
+      <c r="M5" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3647,8 +3665,17 @@
       <c r="G6" s="4">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>2020</v>
+      </c>
+      <c r="L6">
+        <v>31923</v>
+      </c>
+      <c r="M6">
+        <v>426121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3671,8 +3698,17 @@
       <c r="G7" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>2019</v>
+      </c>
+      <c r="L7">
+        <v>30237</v>
+      </c>
+      <c r="M7">
+        <v>390607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3695,8 +3731,17 @@
       <c r="G8" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>2018</v>
+      </c>
+      <c r="L8">
+        <v>29745</v>
+      </c>
+      <c r="M8">
+        <v>372889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3721,8 +3766,17 @@
         <v>7.8657064517532964</v>
       </c>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>2017</v>
+      </c>
+      <c r="L9">
+        <v>28032</v>
+      </c>
+      <c r="M9">
+        <v>329402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>828</v>
       </c>
@@ -3747,11 +3801,106 @@
         <v>6.955301428467501</v>
       </c>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>2016</v>
+      </c>
+      <c r="L10">
+        <v>26609</v>
+      </c>
+      <c r="M10">
+        <v>354080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>2015</v>
+      </c>
+      <c r="L11">
+        <v>26063</v>
+      </c>
+      <c r="M11">
+        <v>347128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>2014</v>
+      </c>
+      <c r="L12">
+        <v>25277</v>
+      </c>
+      <c r="M12">
+        <v>376121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>2013</v>
+      </c>
+      <c r="L13">
+        <v>25492</v>
+      </c>
+      <c r="M13">
+        <v>382638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>2012</v>
+      </c>
+      <c r="L14">
+        <v>25009</v>
+      </c>
+      <c r="M14">
+        <v>376485</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>2011</v>
+      </c>
+      <c r="L15">
+        <v>24490</v>
+      </c>
+      <c r="M15">
+        <v>368183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>2010</v>
+      </c>
+      <c r="L16">
+        <v>24451</v>
+      </c>
+      <c r="M16">
+        <v>267583</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>2006</v>
+      </c>
+      <c r="L17">
+        <v>23000</v>
+      </c>
+      <c r="M17">
+        <v>311000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>2003</v>
+      </c>
+      <c r="L18">
+        <v>24421</v>
+      </c>
+      <c r="M18">
+        <v>327346</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -3759,8 +3908,17 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>2000</v>
+      </c>
+      <c r="L19">
+        <v>25541</v>
+      </c>
+      <c r="M19">
+        <v>363967</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3768,8 +3926,17 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>1995</v>
+      </c>
+      <c r="L20">
+        <v>28447</v>
+      </c>
+      <c r="M20">
+        <v>393723</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3777,8 +3944,17 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>1990</v>
+      </c>
+      <c r="L21">
+        <v>30802</v>
+      </c>
+      <c r="M21">
+        <v>457061</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3787,7 +3963,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3796,7 +3972,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3805,7 +3981,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3841,119 +4017,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>586</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>587</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>588</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>589</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>590</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="79" t="s">
         <v>591</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="58" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="72" t="s">
         <v>603</v>
       </c>
-      <c r="M2" s="58"/>
-      <c r="N2" s="64" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="79" t="s">
         <v>592</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79" t="s">
         <v>593</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64" t="s">
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79" t="s">
         <v>594</v>
       </c>
-      <c r="S2" s="64"/>
-      <c r="T2" s="58" t="s">
+      <c r="S2" s="79"/>
+      <c r="T2" s="72" t="s">
         <v>604</v>
       </c>
-      <c r="U2" s="58"/>
-      <c r="V2" s="64" t="s">
+      <c r="U2" s="72"/>
+      <c r="V2" s="79" t="s">
         <v>595</v>
       </c>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64" t="s">
+      <c r="W2" s="79"/>
+      <c r="X2" s="79" t="s">
         <v>596</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="58" t="s">
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="72" t="s">
         <v>597</v>
       </c>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="64" t="s">
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="79" t="s">
         <v>598</v>
       </c>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64" t="s">
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79" t="s">
         <v>599</v>
       </c>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64" t="s">
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="79" t="s">
         <v>600</v>
       </c>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="58" t="s">
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="72" t="s">
         <v>601</v>
       </c>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="64" t="s">
+      <c r="AI2" s="72"/>
+      <c r="AJ2" s="79" t="s">
         <v>602</v>
       </c>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM2" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN2" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="AO2" s="70" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM2" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN2" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO2" s="61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -4058,7 +4234,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:41" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
@@ -4161,7 +4337,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:41" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
@@ -4268,7 +4444,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:41" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -4377,7 +4553,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:41" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -4484,7 +4660,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:41" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -4710,123 +4886,112 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="66" t="s">
+    <row r="10" spans="1:41" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="73">
+      <c r="B10" s="64">
         <v>0.1019</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="63" t="s">
         <v>891</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>0.18920000000000001</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="63" t="s">
         <v>892</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="64">
         <v>0.1183</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="63" t="s">
         <v>893</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="64">
         <v>0.15240000000000001</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="63" t="s">
         <v>894</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="64">
         <v>7.5600000000000001E-2</v>
       </c>
-      <c r="M10" s="72" t="s">
+      <c r="M10" s="63" t="s">
         <v>895</v>
       </c>
-      <c r="N10" s="73">
+      <c r="N10" s="64">
         <v>0.31709999999999999</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O10" s="63" t="s">
         <v>896</v>
       </c>
-      <c r="P10" s="73">
+      <c r="P10" s="64">
         <v>0.1699</v>
       </c>
-      <c r="Q10" s="72" t="s">
+      <c r="Q10" s="63" t="s">
         <v>897</v>
       </c>
-      <c r="R10" s="73">
+      <c r="R10" s="64">
         <v>7.8799999999999995E-2</v>
       </c>
-      <c r="S10" s="72" t="s">
+      <c r="S10" s="63" t="s">
         <v>898</v>
       </c>
-      <c r="T10" s="73">
+      <c r="T10" s="64">
         <v>0.15179999999999999</v>
       </c>
-      <c r="U10" s="72" t="s">
+      <c r="U10" s="63" t="s">
         <v>899</v>
       </c>
-      <c r="V10" s="73">
+      <c r="V10" s="64">
         <v>0.13270000000000001</v>
       </c>
-      <c r="W10" s="72" t="s">
+      <c r="W10" s="63" t="s">
         <v>900</v>
       </c>
-      <c r="X10" s="73">
+      <c r="X10" s="64">
         <v>0.13159999999999999</v>
       </c>
-      <c r="Y10" s="72" t="s">
+      <c r="Y10" s="63" t="s">
         <v>901</v>
       </c>
       <c r="Z10" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="AB10" s="73">
+      <c r="AB10" s="64">
         <v>9.35E-2</v>
       </c>
-      <c r="AC10" s="72" t="s">
+      <c r="AC10" s="63" t="s">
         <v>902</v>
       </c>
-      <c r="AD10" s="73">
+      <c r="AD10" s="64">
         <v>0.108</v>
       </c>
-      <c r="AE10" s="72" t="s">
+      <c r="AE10" s="63" t="s">
         <v>903</v>
       </c>
-      <c r="AF10" s="73">
+      <c r="AF10" s="64">
         <v>0.1108</v>
       </c>
-      <c r="AG10" s="72" t="s">
+      <c r="AG10" s="63" t="s">
         <v>904</v>
       </c>
       <c r="AH10" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="AJ10" s="73">
+      <c r="AJ10" s="64">
         <v>0.17549999999999999</v>
       </c>
-      <c r="AK10" s="72" t="s">
+      <c r="AK10" s="63" t="s">
         <v>905</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="AD2:AE2"/>
@@ -4834,6 +4999,17 @@
     <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4856,59 +5032,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>605</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="72" t="s">
         <v>606</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72" t="s">
         <v>607</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72" t="s">
         <v>608</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72" t="s">
         <v>611</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>609</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72" t="s">
         <v>610</v>
       </c>
-      <c r="M2" s="58"/>
-    </row>
-    <row r="3" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M2" s="72"/>
+    </row>
+    <row r="3" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -4945,7 +5121,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
@@ -4986,7 +5162,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
@@ -5023,7 +5199,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -5062,7 +5238,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -5101,7 +5277,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -5183,54 +5359,54 @@
         <v>775</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="66" t="s">
+    <row r="10" spans="1:21" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
         <v>828</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="64">
         <v>0.32179999999999997</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="63" t="s">
         <v>688</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>0.1125</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="63" t="s">
         <v>906</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="64">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="63" t="s">
         <v>907</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="64">
         <v>0.125</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="63" t="s">
         <v>908</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="64">
         <v>9.2700000000000005E-2</v>
       </c>
-      <c r="M10" s="72" t="s">
+      <c r="M10" s="63" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="20" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:C2"/>
@@ -5261,104 +5437,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>612</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>562</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>613</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>614</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>615</v>
       </c>
-      <c r="I2" s="64"/>
+      <c r="I2" s="79"/>
       <c r="J2" s="55" t="s">
         <v>616</v>
       </c>
       <c r="K2" s="55"/>
-      <c r="L2" s="64" t="s">
+      <c r="L2" s="79" t="s">
         <v>617</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="79" t="s">
         <v>618</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79" t="s">
         <v>619</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="58" t="s">
+      <c r="Q2" s="79"/>
+      <c r="R2" s="72" t="s">
         <v>630</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="64" t="s">
+      <c r="S2" s="72"/>
+      <c r="T2" s="79" t="s">
         <v>620</v>
       </c>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64" t="s">
+      <c r="U2" s="79"/>
+      <c r="V2" s="79" t="s">
         <v>621</v>
       </c>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64" t="s">
+      <c r="W2" s="79"/>
+      <c r="X2" s="79" t="s">
         <v>622</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64" t="s">
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79" t="s">
         <v>623</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64" t="s">
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79" t="s">
         <v>624</v>
       </c>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64" t="s">
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79" t="s">
         <v>625</v>
       </c>
-      <c r="AE2" s="64"/>
+      <c r="AE2" s="79"/>
       <c r="AF2" s="55" t="s">
         <v>626</v>
       </c>
       <c r="AG2" s="55"/>
-      <c r="AH2" s="64" t="s">
+      <c r="AH2" s="79" t="s">
         <v>627</v>
       </c>
-      <c r="AI2" s="64"/>
-      <c r="AJ2" s="64" t="s">
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79" t="s">
         <v>628</v>
       </c>
-      <c r="AK2" s="64"/>
-      <c r="AL2" s="64" t="s">
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79" t="s">
         <v>629</v>
       </c>
-      <c r="AM2" s="64"/>
-    </row>
-    <row r="3" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AM2" s="79"/>
+    </row>
+    <row r="3" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -5465,7 +5641,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:39" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
@@ -5568,7 +5744,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
@@ -5671,7 +5847,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -5778,7 +5954,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:39" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:39" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -5885,7 +6061,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:39" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -6096,23 +6272,23 @@
         <v>826</v>
       </c>
     </row>
-    <row r="10" spans="1:39" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="66" t="s">
+    <row r="10" spans="1:39" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
         <v>828</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>392</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="64">
         <v>0.13619999999999999</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="64" t="s">
         <v>910</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>9.6799999999999997E-2</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="63" t="s">
         <v>911</v>
       </c>
       <c r="H10" s="29" t="s">
@@ -6124,55 +6300,55 @@
       <c r="K10" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="64">
         <v>0.21790000000000001</v>
       </c>
-      <c r="M10" s="72" t="s">
+      <c r="M10" s="63" t="s">
         <v>912</v>
       </c>
-      <c r="N10" s="73">
+      <c r="N10" s="64">
         <v>6.8900000000000003E-2</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O10" s="63" t="s">
         <v>913</v>
       </c>
       <c r="P10" s="29" t="s">
         <v>392</v>
       </c>
-      <c r="R10" s="73">
+      <c r="R10" s="64">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="S10" s="72" t="s">
+      <c r="S10" s="63" t="s">
         <v>914</v>
       </c>
-      <c r="T10" s="73">
+      <c r="T10" s="64">
         <v>0.12529999999999999</v>
       </c>
-      <c r="U10" s="72" t="s">
+      <c r="U10" s="63" t="s">
         <v>915</v>
       </c>
-      <c r="V10" s="73">
+      <c r="V10" s="64">
         <v>0.16719999999999999</v>
       </c>
-      <c r="W10" s="72" t="s">
+      <c r="W10" s="63" t="s">
         <v>916</v>
       </c>
-      <c r="X10" s="73">
+      <c r="X10" s="64">
         <v>0.1162</v>
       </c>
-      <c r="Y10" s="72" t="s">
+      <c r="Y10" s="63" t="s">
         <v>917</v>
       </c>
-      <c r="Z10" s="73">
+      <c r="Z10" s="64">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="AA10" s="72" t="s">
+      <c r="AA10" s="63" t="s">
         <v>918</v>
       </c>
-      <c r="AB10" s="73">
+      <c r="AB10" s="64">
         <v>0.1547</v>
       </c>
-      <c r="AC10" s="72" t="s">
+      <c r="AC10" s="63" t="s">
         <v>919</v>
       </c>
       <c r="AD10" s="29" t="s">
@@ -6181,76 +6357,76 @@
       <c r="AF10" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="AH10" s="73">
+      <c r="AH10" s="64">
         <v>9.8900000000000002E-2</v>
       </c>
-      <c r="AI10" s="72" t="s">
+      <c r="AI10" s="63" t="s">
         <v>920</v>
       </c>
-      <c r="AJ10" s="73">
+      <c r="AJ10" s="64">
         <v>8.0600000000000005E-2</v>
       </c>
-      <c r="AK10" s="72" t="s">
+      <c r="AK10" s="63" t="s">
         <v>921</v>
       </c>
-      <c r="AL10" s="73">
+      <c r="AL10" s="64">
         <v>0.17460000000000001</v>
       </c>
-      <c r="AM10" s="72" t="s">
+      <c r="AM10" s="63" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="11" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="20" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="22" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="23" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="24" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="25" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="26" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="27" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="28" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="29" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="30" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="31" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="32" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="33" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="34" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="35" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="36" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="37" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="38" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="39" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="40" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="41" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="42" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="30" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="31" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="32" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="33" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="34" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="35" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="36" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="37" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="38" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="39" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="40" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="41" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="42" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6273,64 +6449,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>631</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>632</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>633</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>634</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>635</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="79" t="s">
         <v>636</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="79" t="s">
         <v>637</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="79" t="s">
         <v>638</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79" t="s">
         <v>639</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64" t="s">
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79" t="s">
         <v>640</v>
       </c>
-      <c r="S2" s="64"/>
-    </row>
-    <row r="3" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S2" s="79"/>
+    </row>
+    <row r="3" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -6383,7 +6559,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
@@ -6438,7 +6614,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
@@ -6497,7 +6673,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -6554,7 +6730,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -6613,7 +6789,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -6731,80 +6907,80 @@
         <v>800</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="74" t="s">
+    <row r="10" spans="1:19" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="65" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="73">
+      <c r="B10" s="64">
         <v>0.14660000000000001</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="63" t="s">
         <v>923</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="64">
         <v>0.1565</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="63" t="s">
         <v>924</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>0.1134</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="63" t="s">
         <v>925</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="64">
         <v>7.9500000000000001E-2</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="63" t="s">
         <v>926</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="64">
         <v>8.1500000000000003E-2</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="63" t="s">
         <v>927</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="64">
         <v>6.0400000000000002E-2</v>
       </c>
-      <c r="M10" s="72" t="s">
+      <c r="M10" s="63" t="s">
         <v>928</v>
       </c>
-      <c r="N10" s="73">
+      <c r="N10" s="64">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="O10" s="72" t="s">
+      <c r="O10" s="63" t="s">
         <v>929</v>
       </c>
-      <c r="P10" s="73">
+      <c r="P10" s="64">
         <v>0.18160000000000001</v>
       </c>
-      <c r="Q10" s="72" t="s">
+      <c r="Q10" s="63" t="s">
         <v>930</v>
       </c>
-      <c r="R10" s="73">
+      <c r="R10" s="64">
         <v>8.6099999999999996E-2</v>
       </c>
-      <c r="S10" s="72" t="s">
+      <c r="S10" s="63" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="20" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="22" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="23" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="24" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="25" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="P2:Q2"/>
@@ -6838,44 +7014,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>641</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>642</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>643</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>644</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>645</v>
       </c>
-      <c r="I2" s="64"/>
-    </row>
-    <row r="3" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="79"/>
+    </row>
+    <row r="3" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
         <v>33</v>
       </c>
@@ -6904,7 +7080,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
@@ -6933,7 +7109,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
         <v>35</v>
       </c>
@@ -6962,7 +7138,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
         <v>36</v>
       </c>
@@ -6991,7 +7167,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="27" t="s">
         <v>37</v>
       </c>
@@ -7020,7 +7196,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="27" t="s">
         <v>38</v>
       </c>
@@ -7078,51 +7254,51 @@
         <v>782</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="72" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="66" t="s">
+    <row r="10" spans="1:14" s="63" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="57" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="73">
+      <c r="B10" s="64">
         <v>0.1174</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="63" t="s">
         <v>932</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="64">
         <v>0.1138</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="63" t="s">
         <v>933</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>0.1618</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="63" t="s">
         <v>934</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="64">
         <v>0.1201</v>
       </c>
-      <c r="I10" s="72" t="s">
+      <c r="I10" s="63" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="17" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="18" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="19" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="20" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="21" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="22" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="23" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="24" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="25" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="26" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" s="63" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
@@ -7151,30 +7327,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="59" t="s">
         <v>646</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="72"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
@@ -7254,10 +7430,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="66" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="71">
+      <c r="B10" s="62">
         <v>0.1709</v>
       </c>
       <c r="C10" s="33" t="s">
@@ -7265,8 +7441,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="21"/>
@@ -7316,7 +7492,7 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -7329,18 +7505,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="71"/>
+      <c r="D1" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="71"/>
+      <c r="F1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="57"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -7527,7 +7703,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="69" t="s">
         <v>828</v>
       </c>
       <c r="B10" s="8">
@@ -7579,25 +7755,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="74" t="s">
         <v>676</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="72" t="s">
         <v>673</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72" t="s">
         <v>674</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="61"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="75"/>
       <c r="G1" s="41"/>
       <c r="H1" s="36"/>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="60"/>
+      <c r="A2" s="74"/>
       <c r="B2" s="44" t="s">
         <v>675</v>
       </c>
@@ -7610,7 +7786,7 @@
       <c r="E2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="41"/>
       <c r="H2" s="36"/>
       <c r="I2" s="19"/>
@@ -8119,18 +8295,18 @@
     <row r="25" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37"/>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="72" t="s">
         <v>673</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58" t="s">
+      <c r="C27" s="72"/>
+      <c r="D27" s="72" t="s">
         <v>674</v>
       </c>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59" t="s">
+      <c r="E27" s="72"/>
+      <c r="F27" s="73" t="s">
         <v>677</v>
       </c>
-      <c r="G27" s="59"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -8213,13 +8389,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="12"/>
-    <col min="2" max="2" width="10" style="77" customWidth="1"/>
+    <col min="2" max="2" width="10" style="67" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="14"/>
-    <col min="4" max="4" width="10.83203125" style="77"/>
+    <col min="4" max="4" width="10.83203125" style="67"/>
     <col min="5" max="5" width="10.83203125" style="14"/>
-    <col min="6" max="6" width="10.83203125" style="77"/>
+    <col min="6" max="6" width="10.83203125" style="67"/>
     <col min="7" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="10.83203125" style="77"/>
+    <col min="8" max="8" width="10.83203125" style="67"/>
     <col min="9" max="9" width="10.83203125" style="14"/>
     <col min="10" max="16384" width="10.83203125" style="12"/>
   </cols>
@@ -8249,25 +8425,25 @@
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="67" t="s">
         <v>678</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>679</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="67" t="s">
         <v>678</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>679</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="67" t="s">
         <v>678</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>679</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="67" t="s">
         <v>678</v>
       </c>
       <c r="I2" s="14" t="s">
@@ -8281,28 +8457,28 @@
       <c r="A3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="67">
         <f t="shared" ref="B3:B8" si="0">$J3*C3%</f>
         <v>76.239999999999995</v>
       </c>
       <c r="C3" s="14">
         <v>8</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="67">
         <f>$J3*E3%</f>
         <v>458.39300000000003</v>
       </c>
       <c r="E3" s="14">
         <v>48.1</v>
       </c>
-      <c r="F3" s="77">
+      <c r="F3" s="67">
         <f>$J3*G3%</f>
         <v>211.566</v>
       </c>
       <c r="G3" s="14">
         <v>22.2</v>
       </c>
-      <c r="H3" s="77">
+      <c r="H3" s="67">
         <f t="shared" ref="H3:H8" si="1">$J3*I3%</f>
         <v>206.80099999999999</v>
       </c>
@@ -8312,215 +8488,215 @@
       <c r="J3" s="12">
         <v>953</v>
       </c>
-      <c r="K3" s="77"/>
+      <c r="K3" s="67"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="77">
+      <c r="B4" s="67">
         <f t="shared" si="0"/>
         <v>193.55600000000001</v>
       </c>
       <c r="C4" s="14">
         <v>16.600000000000001</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="67">
         <f>$J4*E4%</f>
         <v>513.04</v>
       </c>
       <c r="E4" s="14">
         <v>44</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="67">
         <f>$J4*G4%</f>
         <v>180.73</v>
       </c>
       <c r="G4" s="14">
         <v>15.5</v>
       </c>
-      <c r="H4" s="77">
+      <c r="H4" s="67">
         <f t="shared" si="1"/>
         <v>278.67399999999998</v>
       </c>
       <c r="I4" s="14">
         <v>23.9</v>
       </c>
-      <c r="J4" s="77">
+      <c r="J4" s="67">
         <v>1166</v>
       </c>
-      <c r="K4" s="77"/>
+      <c r="K4" s="67"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="77">
+      <c r="B5" s="67">
         <f t="shared" si="0"/>
         <v>62.712000000000003</v>
       </c>
       <c r="C5" s="14">
         <v>5.2</v>
       </c>
-      <c r="D5" s="77">
+      <c r="D5" s="67">
         <f>$J5*E5%</f>
         <v>490.84200000000004</v>
       </c>
       <c r="E5" s="14">
         <v>40.700000000000003</v>
       </c>
-      <c r="F5" s="77">
+      <c r="F5" s="67">
         <f>$J5*G5%</f>
         <v>399.18600000000004</v>
       </c>
       <c r="G5" s="14">
         <v>33.1</v>
       </c>
-      <c r="H5" s="77">
+      <c r="H5" s="67">
         <f t="shared" si="1"/>
         <v>253.26</v>
       </c>
       <c r="I5" s="14">
         <v>21</v>
       </c>
-      <c r="J5" s="77">
+      <c r="J5" s="67">
         <v>1206</v>
       </c>
-      <c r="K5" s="77"/>
+      <c r="K5" s="67"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="77">
+      <c r="B6" s="67">
         <f t="shared" si="0"/>
         <v>160.13999999999999</v>
       </c>
       <c r="C6" s="14">
         <v>10.199999999999999</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="67">
         <v>743</v>
       </c>
       <c r="E6" s="14">
         <v>47.4</v>
       </c>
-      <c r="F6" s="77">
+      <c r="F6" s="67">
         <f>$J6*G6%</f>
         <v>395.64</v>
       </c>
       <c r="G6" s="14">
         <v>25.2</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="67">
         <f t="shared" si="1"/>
         <v>271.61</v>
       </c>
       <c r="I6" s="14">
         <v>17.3</v>
       </c>
-      <c r="J6" s="77">
+      <c r="J6" s="67">
         <v>1570</v>
       </c>
-      <c r="K6" s="77"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="77">
+      <c r="B7" s="67">
         <f t="shared" si="0"/>
         <v>72.335999999999999</v>
       </c>
       <c r="C7" s="14">
         <v>6.6</v>
       </c>
-      <c r="D7" s="77">
+      <c r="D7" s="67">
         <v>529</v>
       </c>
       <c r="E7" s="14">
         <v>48.4</v>
       </c>
-      <c r="F7" s="77">
+      <c r="F7" s="67">
         <f>$J7*G7%</f>
         <v>332.08799999999997</v>
       </c>
       <c r="G7" s="14">
         <v>30.3</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="67">
         <f t="shared" si="1"/>
         <v>162.20800000000003</v>
       </c>
       <c r="I7" s="14">
         <v>14.8</v>
       </c>
-      <c r="J7" s="77">
+      <c r="J7" s="67">
         <v>1096</v>
       </c>
-      <c r="K7" s="77"/>
+      <c r="K7" s="67"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="77">
+      <c r="B8" s="67">
         <f t="shared" si="0"/>
         <v>95.108000000000004</v>
       </c>
       <c r="C8" s="14">
         <v>6.2</v>
       </c>
-      <c r="D8" s="77">
+      <c r="D8" s="67">
         <v>587</v>
       </c>
       <c r="E8" s="14">
         <v>38.299999999999997</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="67">
         <v>389</v>
       </c>
       <c r="G8" s="14">
         <v>25.4</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="67">
         <f t="shared" si="1"/>
         <v>463.26799999999997</v>
       </c>
       <c r="I8" s="14">
         <v>30.2</v>
       </c>
-      <c r="J8" s="77">
+      <c r="J8" s="67">
         <v>1534</v>
       </c>
-      <c r="K8" s="77"/>
+      <c r="K8" s="67"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="68">
         <v>127</v>
       </c>
       <c r="C9" s="14">
         <f>B9*100/$J$9</f>
         <v>10.444078947368421</v>
       </c>
-      <c r="D9" s="78">
+      <c r="D9" s="68">
         <v>570</v>
       </c>
       <c r="E9" s="14">
         <f>D9*100/$J$9</f>
         <v>46.875</v>
       </c>
-      <c r="F9" s="78">
+      <c r="F9" s="68">
         <v>354</v>
       </c>
       <c r="G9" s="14">
         <f>F9*100/$J$9</f>
         <v>29.111842105263158</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="68">
         <v>165</v>
       </c>
       <c r="I9" s="14">
@@ -8531,31 +8707,31 @@
         <f>B9+D9+F9+H9</f>
         <v>1216</v>
       </c>
-      <c r="K9" s="77"/>
+      <c r="K9" s="67"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="58" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="77">
+      <c r="B10" s="67">
         <v>143</v>
       </c>
       <c r="C10" s="14">
         <v>12.2</v>
       </c>
-      <c r="D10" s="77">
+      <c r="D10" s="67">
         <v>567</v>
       </c>
       <c r="E10" s="14">
         <v>48.3</v>
       </c>
-      <c r="F10" s="77">
+      <c r="F10" s="67">
         <v>324</v>
       </c>
       <c r="G10" s="14">
         <v>27.6</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="67">
         <v>141</v>
       </c>
       <c r="I10" s="14">
@@ -8565,7 +8741,7 @@
         <f>B10+D10+F10+H10</f>
         <v>1175</v>
       </c>
-      <c r="K10" s="77"/>
+      <c r="K10" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8605,11 +8781,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
@@ -8940,46 +9116,46 @@
       <c r="A1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63" t="s">
+      <c r="E1" s="78"/>
+      <c r="F1" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63" t="s">
+      <c r="G1" s="78"/>
+      <c r="H1" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63" t="s">
+      <c r="I1" s="78"/>
+      <c r="J1" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63" t="s">
+      <c r="K1" s="78"/>
+      <c r="L1" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63" t="s">
+      <c r="M1" s="78"/>
+      <c r="N1" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63" t="s">
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="78"/>
+      <c r="T1" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="63"/>
+      <c r="U1" s="78"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -9518,16 +9694,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9551,67 +9727,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="70" t="s">
         <v>546</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72" t="s">
         <v>544</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72" t="s">
         <v>538</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72" t="s">
         <v>539</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>540</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72" t="s">
         <v>545</v>
       </c>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>541</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72" t="s">
         <v>542</v>
       </c>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58" t="s">
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="S2" s="58"/>
+      <c r="S2" s="72"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
@@ -10091,46 +10267,46 @@
       <c r="A2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="72" t="s">
         <v>549</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72" t="s">
         <v>551</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>557</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58" t="s">
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72" t="s">
         <v>553</v>
       </c>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58" t="s">
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58" t="s">
+      <c r="S2" s="72"/>
+      <c r="T2" s="72" t="s">
         <v>555</v>
       </c>
-      <c r="U2" s="58"/>
+      <c r="U2" s="72"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
@@ -10577,7 +10753,7 @@
       <c r="A10" s="31" t="s">
         <v>828</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="56" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="29"/>
@@ -10716,106 +10892,106 @@
       <c r="A2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="79" t="s">
         <v>560</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>561</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="79" t="s">
         <v>563</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="79" t="s">
         <v>564</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64" t="s">
+      <c r="K2" s="79"/>
+      <c r="L2" s="79" t="s">
         <v>565</v>
       </c>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="79" t="s">
         <v>566</v>
       </c>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79" t="s">
         <v>567</v>
       </c>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="58" t="s">
+      <c r="Q2" s="79"/>
+      <c r="R2" s="72" t="s">
         <v>581</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="64" t="s">
+      <c r="S2" s="72"/>
+      <c r="T2" s="79" t="s">
         <v>568</v>
       </c>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64" t="s">
+      <c r="U2" s="79"/>
+      <c r="V2" s="79" t="s">
         <v>569</v>
       </c>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64" t="s">
+      <c r="W2" s="79"/>
+      <c r="X2" s="79" t="s">
         <v>570</v>
       </c>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64" t="s">
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64" t="s">
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79" t="s">
         <v>572</v>
       </c>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64" t="s">
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79" t="s">
         <v>573</v>
       </c>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64" t="s">
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="79" t="s">
         <v>574</v>
       </c>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="58" t="s">
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="72" t="s">
         <v>575</v>
       </c>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="58" t="s">
+      <c r="AI2" s="72"/>
+      <c r="AJ2" s="72" t="s">
         <v>582</v>
       </c>
-      <c r="AK2" s="58"/>
-      <c r="AL2" s="64" t="s">
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="79" t="s">
         <v>576</v>
       </c>
-      <c r="AM2" s="64"/>
+      <c r="AM2" s="79"/>
       <c r="AN2" s="32" t="s">
         <v>583</v>
       </c>
       <c r="AO2" s="32"/>
-      <c r="AP2" s="58" t="s">
+      <c r="AP2" s="72" t="s">
         <v>584</v>
       </c>
-      <c r="AQ2" s="58"/>
+      <c r="AQ2" s="72"/>
       <c r="AR2" s="30" t="s">
         <v>577</v>
       </c>
       <c r="AS2" s="30"/>
-      <c r="AT2" s="58" t="s">
+      <c r="AT2" s="72" t="s">
         <v>585</v>
       </c>
-      <c r="AU2" s="58"/>
-      <c r="AV2" s="64" t="s">
+      <c r="AU2" s="72"/>
+      <c r="AV2" s="79" t="s">
         <v>578</v>
       </c>
-      <c r="AW2" s="64"/>
-      <c r="AX2" s="64" t="s">
+      <c r="AW2" s="79"/>
+      <c r="AX2" s="79" t="s">
         <v>579</v>
       </c>
-      <c r="AY2" s="64"/>
+      <c r="AY2" s="79"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
@@ -12018,6 +12194,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="AV2:AW2"/>
     <mergeCell ref="AX2:AY2"/>
@@ -12034,13 +12217,6 @@
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>